<commit_message>
Create Admin Auditor using Mongodb service
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="16" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -16,29 +16,30 @@
     <sheet name="authSessions" sheetId="9" r:id="rId7"/>
     <sheet name="ForgotPassword" sheetId="2" r:id="rId8"/>
     <sheet name="Login" sheetId="3" r:id="rId9"/>
-    <sheet name="usersRegression" sheetId="10" r:id="rId10"/>
-    <sheet name="EmailTemplateData" sheetId="13" r:id="rId11"/>
-    <sheet name="ClientTestData" sheetId="12" r:id="rId12"/>
-    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId13"/>
-    <sheet name="ClientUITest" sheetId="20" r:id="rId14"/>
-    <sheet name="TodoTestPage" sheetId="16" r:id="rId15"/>
-    <sheet name="SuperAdminTest" sheetId="17" r:id="rId16"/>
-    <sheet name="NotificationEmailTest" sheetId="18" r:id="rId17"/>
-    <sheet name="ClientSignUpTest" sheetId="19" r:id="rId18"/>
-    <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId19"/>
-    <sheet name="SmokeTest" sheetId="14" r:id="rId20"/>
-    <sheet name="SmokeTest-R" sheetId="25" r:id="rId21"/>
-    <sheet name="GroupPermissionTest" sheetId="24" r:id="rId22"/>
+    <sheet name="EmailTemplateData" sheetId="13" r:id="rId10"/>
+    <sheet name="ClientTestData" sheetId="12" r:id="rId11"/>
+    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId12"/>
+    <sheet name="ClientUITest" sheetId="20" r:id="rId13"/>
+    <sheet name="TodoTestPage" sheetId="16" r:id="rId14"/>
+    <sheet name="SuperAdminTest" sheetId="17" r:id="rId15"/>
+    <sheet name="NotificationEmailTest" sheetId="18" r:id="rId16"/>
+    <sheet name="ClientSignUpTest" sheetId="19" r:id="rId17"/>
+    <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId18"/>
+    <sheet name="SmokeTest" sheetId="14" r:id="rId19"/>
+    <sheet name="SmokeTest-R" sheetId="25" r:id="rId20"/>
+    <sheet name="GroupPermissionTest" sheetId="24" r:id="rId21"/>
+    <sheet name="usersRegression" sheetId="10" r:id="rId22"/>
+    <sheet name="SetupUserRoles" sheetId="26" r:id="rId23"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="11" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="12" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="21" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="15" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="18" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="653">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2297,6 +2298,126 @@
   <si>
     <t>{"role" : "FIRM_ADMIN",    "priority" : 7,    "__v" : 0}</t>
   </si>
+  <si>
+    <t>AUDITOR</t>
+  </si>
+  <si>
+    <t>Firm User role mapping Json</t>
+  </si>
+  <si>
+    <t>adm.auditorthuan@vietnam-software.org</t>
+  </si>
+  <si>
+    <t>59db42c0e87847296323fa8b</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db42c0e87847296323fa8d"},
+    "userID" : { "$oid" : "59db42c0e87847296323fa8b"},
+    "firmID" : { "$oid" : "59db42c0e87847296323fa8c"},
+    "role" : "FIRM_ADMIN",
+    "priority" : 7,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db42c0e87847296323fa8b"},
+    "email" : "adm.auditorthuan@vietnam-software.org",
+    "type" : "AUDITOR",
+    "status" : "ACTIVE",
+    "locale" : "en-US",
+    "notification" : {
+        "SMSVerified" : false,
+        "SMSEnabled" : false,
+        "day" : null,
+        "time" : null,
+        "frequency" : "IMMEDIATELY",
+        "content" : "JUSTME"
+    },
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "passwordLockout" : {
+        "expires" : null,
+        "failedAttempts" : 0
+    },
+    "auth" : {
+        "id" : "AvaE2jva4TK5-YnTPy5KIEQJM",
+        "access" : {
+            "expires" : {"$date":"2017-10-10T02:50:38.521Z"}
+        }
+    },
+    "referral" : "Conference",
+    "agreements" : [],
+    "integrations" : [],
+    "verified" : true,
+    "passwordResetRequired" : false,
+    "lastOnboardedEID" : "",
+    "skipOnboard" : true,
+    "lastLogin" : {"$date":"2017-10-10T02:50:42.484Z"},
+    "dateCreated" : {"$date":"2017-10-09T11:52:19.120Z"},
+    "phone" : "123-456-7890",
+    "jobTitle" : "Managing Partner",
+    "lastName" : "Auditor",
+    "firstName" : "Admin",
+    "password_salt" : "$2a$10$BqKA70C3TgE/.nHVMUIgxe",
+    "password" : "$2a$10$BqKA70C3TgE/.nHVMUIgxedjl68sQa3f24mkvW92c3mDlF8ZVA1.m",
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db42c0e87847296323fa8c"},
+    "name" : "Firm Auvenir1",
+    "address" : {
+        "country" : "CA",
+        "postalCode" : "K3G4P8",
+        "stateProvince" : "Quebec",
+        "city" : "Toronto",
+        "streetAddress" : "123 Hoang Van Thu",
+        "unit" : "12345"
+    },
+    "memberID" : "3215",
+    "previousName" : "",
+    "nameChange" : false,
+    "logoDisplayAgreed" : false,
+    "affiliatedFirms" : [],
+    "affiliated" : false,
+    "phone" : "123456-7890",
+    "size" : "1",
+    "website" : "titancorpvn.com",
+    "logo" : "",
+    "acl" : [],
+    "__v" : 2
+}</t>
+  </si>
+  <si>
+    <t>59db42c0e87847296323fa8c</t>
+  </si>
+  <si>
+    <t>firmID</t>
+  </si>
 </sst>
 </file>
 
@@ -2508,7 +2629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2664,6 +2785,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2671,9 +2795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2687,6 +2808,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3320,289 +3447,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="8" width="26" style="75" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="28.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" style="75" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F1" s="48" t="s">
-        <v>227</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>634</v>
-      </c>
-      <c r="H1" s="48" t="s">
-        <v>635</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>226</v>
-      </c>
-      <c r="J1" s="48" t="s">
-        <v>225</v>
-      </c>
-      <c r="K1" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="L1" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="M1" t="s">
-        <v>222</v>
-      </c>
-      <c r="N1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O1" s="48" t="s">
-        <v>642</v>
-      </c>
-      <c r="P1" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="48" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
-        <v>504</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>557</v>
-      </c>
-      <c r="C2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" t="s">
-        <v>636</v>
-      </c>
-      <c r="G2" s="75" t="s">
-        <v>639</v>
-      </c>
-      <c r="H2" s="75" t="s">
-        <v>638</v>
-      </c>
-      <c r="I2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J2" t="s">
-        <v>217</v>
-      </c>
-      <c r="K2" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" t="s">
-        <v>215</v>
-      </c>
-      <c r="M2" s="37" t="s">
-        <v>632</v>
-      </c>
-      <c r="N2" t="s">
-        <v>214</v>
-      </c>
-      <c r="O2" s="75" t="s">
-        <v>643</v>
-      </c>
-      <c r="P2" t="s">
-        <v>549</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
-        <v>505</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>503</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F3" t="s">
-        <v>640</v>
-      </c>
-      <c r="G3" s="75" t="s">
-        <v>641</v>
-      </c>
-      <c r="H3" s="75" t="s">
-        <v>637</v>
-      </c>
-      <c r="I3" t="s">
-        <v>207</v>
-      </c>
-      <c r="J3" t="s">
-        <v>211</v>
-      </c>
-      <c r="K3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L3" t="s">
-        <v>209</v>
-      </c>
-      <c r="M3" s="37" t="s">
-        <v>633</v>
-      </c>
-      <c r="N3" t="s">
-        <v>208</v>
-      </c>
-      <c r="O3" s="75" t="s">
-        <v>643</v>
-      </c>
-      <c r="P3" s="59" t="s">
-        <v>549</v>
-      </c>
-      <c r="Q3" s="59" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="47"/>
-      <c r="M4" s="77"/>
-    </row>
-    <row r="5" spans="1:28" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="47"/>
-      <c r="F6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
-      <c r="Z6" s="59"/>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="59"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="70"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="47"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3709,7 +3553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -3784,7 +3628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -3851,7 +3695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -4118,7 +3962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
@@ -4295,7 +4139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -4426,7 +4270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -4629,7 +4473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4675,7 +4519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
@@ -5559,109 +5403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="K1" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="L1" s="39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA10"/>
   <sheetViews>
@@ -5969,7 +5711,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
@@ -6996,11 +6840,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection sqref="A1:D98"/>
     </sheetView>
   </sheetViews>
@@ -7970,6 +7814,476 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB22"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="8" width="26" style="75" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="13" width="28.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" style="75" customWidth="1"/>
+    <col min="17" max="17" width="32.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>634</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>635</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="M1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>642</v>
+      </c>
+      <c r="P1" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="48" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>504</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>557</v>
+      </c>
+      <c r="C2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" t="s">
+        <v>636</v>
+      </c>
+      <c r="G2" s="75" t="s">
+        <v>639</v>
+      </c>
+      <c r="H2" s="75" t="s">
+        <v>638</v>
+      </c>
+      <c r="I2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" t="s">
+        <v>215</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>632</v>
+      </c>
+      <c r="N2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="75" t="s">
+        <v>643</v>
+      </c>
+      <c r="P2" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>505</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" t="s">
+        <v>640</v>
+      </c>
+      <c r="G3" s="75" t="s">
+        <v>641</v>
+      </c>
+      <c r="H3" s="75" t="s">
+        <v>637</v>
+      </c>
+      <c r="I3" t="s">
+        <v>207</v>
+      </c>
+      <c r="J3" t="s">
+        <v>211</v>
+      </c>
+      <c r="K3" t="s">
+        <v>210</v>
+      </c>
+      <c r="L3" t="s">
+        <v>209</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>633</v>
+      </c>
+      <c r="N3" t="s">
+        <v>208</v>
+      </c>
+      <c r="O3" s="75" t="s">
+        <v>643</v>
+      </c>
+      <c r="P3" s="59" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q3" s="59" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="47"/>
+      <c r="M4" s="77"/>
+    </row>
+    <row r="5" spans="1:28" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="47"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B6" s="47"/>
+      <c r="F6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
+      <c r="Z6" s="59"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B7" s="70"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B8" s="47"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B10" s="47"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B12" s="47"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B15" s="47"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B16" s="47"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="47"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="47"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="37"/>
+    <col min="5" max="5" width="9.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" style="37" customWidth="1"/>
+    <col min="10" max="10" width="20" style="37" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" style="37" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="37" customWidth="1"/>
+    <col min="13" max="13" width="21" style="37" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="87" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="87" t="s">
+        <v>634</v>
+      </c>
+      <c r="H1" s="87" t="s">
+        <v>652</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="K1" s="87" t="s">
+        <v>645</v>
+      </c>
+      <c r="L1" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="87" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>504</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>557</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>636</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>639</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>638</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>632</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>643</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>549</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>505</v>
+      </c>
+      <c r="B3" s="88" t="s">
+        <v>503</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>641</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>637</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>633</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="K3" s="37" t="s">
+        <v>643</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>549</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>509</v>
+      </c>
+      <c r="B4" s="88" t="s">
+        <v>646</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>644</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>647</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>651</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>649</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>650</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>648</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8698,22 +9012,22 @@
       <c r="Q1" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="82" t="s">
+      <c r="R1" s="79" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="82"/>
-      <c r="T1" s="81" t="s">
+      <c r="S1" s="79"/>
+      <c r="T1" s="82" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="79"/>
-      <c r="V1" s="82" t="s">
+      <c r="U1" s="80"/>
+      <c r="V1" s="79" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="79" t="s">
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="80" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="83" t="s">
@@ -8765,8 +9079,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="80"/>
-      <c r="AB2" s="80"/>
+      <c r="AA2" s="81"/>
+      <c r="AB2" s="81"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -8822,6 +9136,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -8832,17 +9157,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add 6 roles in database
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="689">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2308,9 +2308,6 @@
     <t>adm.auditorthuan@vietnam-software.org</t>
   </si>
   <si>
-    <t>59db42c0e87847296323fa8b</t>
-  </si>
-  <si>
     <t>{
     "_id" : { "$oid" : "59db42c0e87847296323fa8d"},
     "userID" : { "$oid" : "59db42c0e87847296323fa8b"},
@@ -2387,6 +2384,9 @@
 }</t>
   </si>
   <si>
+    <t>Engagement1 Json</t>
+  </si>
+  <si>
     <t>{
     "_id" : { "$oid" : "59db42c0e87847296323fa8c"},
     "name" : "Firm Auvenir1",
@@ -2408,15 +2408,786 @@
     "size" : "1",
     "website" : "titancorpvn.com",
     "logo" : "",
-    "acl" : [],
+    "acl" : [
+     {
+            "id" : { "$oid" : "59db42c0e87847296323fa8b"},
+            "admin" : true
+        }, 
+        {
+            "id" : { "$oid" : "59db432ee87847296323fa94"},
+            "admin" : false
+        }, 
+        {
+            "id" : { "$oid" : "59db4405e87847296323faaf"},
+            "admin" : false
+        }
+ ],
     "__v" : 2
 }</t>
   </si>
   <si>
-    <t>59db42c0e87847296323fa8c</t>
-  </si>
-  <si>
-    <t>firmID</t>
+    <t>{
+    "_id" : { "$oid" : "59db4308e87847296323fa90"},
+    "status" : "ACTIVE",
+    "previousStatus" : "ACTIVE",
+    "dueDate" : {"$date":"2017-10-18T17:00:00.000Z"},
+    "dateCompleted" : null,
+    "lastUpdated" : null,
+    "dateCreated" : {"$date":"2017-10-09T11:52:40.985Z"},
+    "categories" : [],
+    "bankStatementDateRange" : {
+        "startDate" : {"$date":"2017-10-08T17:00:00.000Z"},
+        "endDate" : {"$date":"2017-10-18T17:00:00.000Z"}
+    },
+    "firm" : {
+        "id" : { "$oid" : "59db42c0e87847296323fa8c"},
+        "creater" : { "$oid" : "59db42c0e87847296323fa8b"},
+        "currentOwner" : { "$oid" : "59db42c0e87847296323fa8b"}
+    },
+    "name" : "Engagement GP01",
+    "acl" : [
+  {
+            "id" : { "$oid" : "59db42c0e87847296323fa8b"},
+            "role" : "AUDITOR",
+            "status" : "ACTIVE",
+            "lead" : true
+        },
+  {
+            "role" : "AUDITOR",
+            "id" : { "$oid" : "59db432ee87847296323fa94"},
+            "status" : "ACTIVE",
+            "lead" : false
+        }, 
+        {
+            "role" : "CLIENT",
+            "id" : { "$oid" : "59db4373e87847296323fa9b"},
+            "status" : "ACTIVE",
+            "lead" : true
+        }
+ ],
+    "__v" : 2,
+    "business" : {
+        "id" : { "$oid" : "59db4308e87847296323fa8f"},
+        "keyContact" : { "$oid" : "59db4373e87847296323fa9b"}
+    },
+    "type" : "Review"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4308e87847296323fa8f"},
+    "name" : "Titan",
+    "address" : {
+        "country" : "",
+        "postalCode" : "",
+        "stateProvince" : "",
+        "city" : "",
+        "streetAddress" : "",
+        "unit" : ""
+    },
+    "parentStakeholders" : "",
+    "overseasOps" : false,
+    "publiclyListed" : false,
+    "previousLegalName" : "",
+    "legalNameChanged" : false,
+    "fiscalYearEnd" : {"$date":"1970-01-27T17:00:00.000Z"},
+    "accountingFramework" : "ASPE",
+    "timezone" : "",
+    "website" : "",
+    "industry" : "Agriculture, Forestry, Fishing and Hunting",
+    "acl" : [ 
+        {
+            "id" : { "$oid" : "59db4373e87847296323fa9b"},
+            "admin" : true
+        }, 
+        {
+            "id" : { "$oid" : "59db444fe87847296323fab8"},
+            "admin" : false
+        }, 
+        {
+            "id" : { "$oid" : "59db44b4e87847296323fac4"},
+            "admin" : false
+        }
+    ],
+    "__v" : 3
+}</t>
+  </si>
+  <si>
+    <t>Business Json</t>
+  </si>
+  <si>
+    <t>lead.auditorthuan@vietnam-software.org</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db432ee87847296323fa94"},
+    "email" : "lead.auditorthuan@vietnam-software.org",
+    "type" : "AUDITOR",
+    "status" : "ACTIVE",
+    "locale" : "en-US",
+    "notification" : {
+        "SMSVerified" : false,
+        "SMSEnabled" : false,
+        "day" : null,
+        "time" : null,
+        "frequency" : "IMMEDIATELY",
+        "content" : "JUSTME"
+    },
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "passwordLockout" : {
+        "expires" : null,
+        "failedAttempts" : 0
+    },
+    "auth" : {
+        "id" : "FvJei1uLB3Dk-vfV6UNQbFMx1",
+        "access" : {
+            "expires" : {"$date":"2017-10-11T04:27:03.115Z"}
+        }
+    },
+    "referral" : "Conference",
+    "agreements" : [ 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:53:23.666Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:53:23.666Z"}
+        }, 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:53:23.666Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:53:23.666Z"}
+        }
+    ],
+    "integrations" : [],
+    "verified" : false,
+    "passwordResetRequired" : false,
+    "lastOnboardedEID" : "",
+    "skipOnboard" : false,
+    "lastLogin" : {"$date":"2017-10-11T04:27:07.165Z"},
+    "dateCreated" : {"$date":"2017-10-09T11:53:51.258Z"},
+    "phone" : "123-456-7899",
+    "jobTitle" : "Partner",
+    "lastName" : "Auditor",
+    "firstName" : "Lead",
+    "password_salt" : "$2a$10$10VBgbzwKpryQfGlE1x58e",
+    "password" : "$2a$10$10VBgbzwKpryQfGlE1x58epNYDUL9f5ornoBPDagLQOxbf0MVMB6K",
+    "__v" : 1
+}</t>
+  </si>
+  <si>
+    <t>Engagement1 role mapping Json</t>
+  </si>
+  <si>
+    <t>Engagement2 role mapping Json</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db432ee87847296323fa96"},
+    "userID" : { "$oid" : "59db432ee87847296323fa94"},
+    "firmID" : { "$oid" : "59db42c0e87847296323fa8c"},
+    "role" : "FIRM_USER",
+    "priority" : 8,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>Engagement2 Json</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db432ee87847296323fa95"},
+    "userID" : { "$oid" : "59db432ee87847296323fa94"},
+    "engagementID" : { "$oid" : "59db4308e87847296323fa90"},
+    "role" : "GENERAL_AUDITOR",
+    "priority" : 2,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db43b0e87847296323faa5"},
+    "userID" : { "$oid" : "59db432ee87847296323fa94"},
+    "engagementID" : { "$oid" : "59db43b0e87847296323faa4"},
+    "role" : "LEAD_AUDITOR",
+    "priority" : 1,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4308e87847296323fa91"},
+    "userID" : { "$oid" : "59db42c0e87847296323fa8b"},
+    "engagementID" : { "$oid" : "59db4308e87847296323fa90"},
+    "role" : "LEAD_AUDITOR",
+    "priority" : 1,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db43b0e87847296323faa6"},
+    "userID" : { "$oid" : "59db42c0e87847296323fa8b"},
+    "engagementID" : { "$oid" : "59db43b0e87847296323faa4"},
+    "role" : "FIRM_ADMIN",
+    "priority" : 7,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4308e87847296323fa92"},
+    "userID" : { "$oid" : "59db42c0e87847296323fa8b"},
+    "engagementID" : { "$oid" : "59db4308e87847296323fa90"},
+    "role" : "FIRM_ADMIN",
+    "priority" : 7,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db43b0e87847296323faa4"},
+    "status" : "ACTIVE",
+    "previousStatus" : "ACTIVE",
+    "dueDate" : {"$date":"2017-10-18T17:00:00.000Z"},
+    "dateCompleted" : null,
+    "lastUpdated" : null,
+    "dateCreated" : {"$date":"2017-10-09T11:55:28.910Z"},
+    "categories" : [],
+    "bankStatementDateRange" : {
+        "startDate" : {"$date":"2017-10-08T17:00:00.000Z"},
+        "endDate" : {"$date":"2017-10-18T17:00:00.000Z"}
+    },
+    "firm" : {
+        "id" : { "$oid" : "59db42c0e87847296323fa8c"},
+        "creater" : { "$oid" : "59db432ee87847296323fa94"},
+        "currentOwner" : { "$oid" : "59db432ee87847296323fa94"}
+    },
+    "name" : "Engagement GP02",
+    "acl" : [ 
+        {
+            "id" : { "$oid" : "59db432ee87847296323fa94"},
+            "role" : "AUDITOR",
+            "status" : "ACTIVE",
+            "lead" : true
+        }, 
+        {
+            "role" : "CLIENT",
+            "id" : { "$oid" : "59db4373e87847296323fa9b"},
+            "status" : "INACTIVE",
+            "lead" : false
+        }, 
+        {
+            "role" : "AUDITOR",
+            "id" : { "$oid" : "59db4405e87847296323faaf"},
+            "status" : "ACTIVE",
+            "lead" : false
+        }, 
+        {
+            "role" : "CLIENT",
+            "id" : { "$oid" : "59db444fe87847296323fab8"},
+            "status" : "ACTIVE",
+            "lead" : true
+        }, 
+        {
+            "role" : "CLIENT",
+            "id" : { "$oid" : "59db44b4e87847296323fac4"},
+            "status" : "ACTIVE",
+            "lead" : false
+        }
+    ],
+    "__v" : 4,
+    "business" : {
+        "id" : { "$oid" : "59db4308e87847296323fa8f"},
+        "keyContact" : { "$oid" : "59db4373e87847296323fa9b"}
+    },
+    "type" : "Review"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4405e87847296323faaf"},
+    "email" : "general.auditorthuan@vietnam-software.org",
+    "type" : "AUDITOR",
+    "status" : "ACTIVE",
+    "locale" : "en-US",
+    "notification" : {
+        "SMSVerified" : false,
+        "SMSEnabled" : false,
+        "day" : null,
+        "time" : null,
+        "frequency" : "IMMEDIATELY",
+        "content" : "JUSTME"
+    },
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "passwordLockout" : {
+        "expires" : null,
+        "failedAttempts" : 0
+    },
+    "auth" : {
+        "id" : "eNoCXf2UbYIA-MnA3HpdUCKCx",
+        "access" : {
+            "expires" : {"$date":"2017-10-09T11:57:05.036Z"}
+        }
+    },
+    "referral" : "Conference",
+    "agreements" : [ 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:57:00.677Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:57:00.677Z"}
+        }, 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:57:00.677Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:57:00.677Z"}
+        }
+    ],
+    "integrations" : [],
+    "verified" : false,
+    "passwordResetRequired" : false,
+    "lastOnboardedEID" : "",
+    "skipOnboard" : false,
+    "lastLogin" : {"$date":"2017-10-09T11:57:08.361Z"},
+    "dateCreated" : {"$date":"2017-10-09T11:57:28.379Z"},
+    "phone" : "123-456-7899",
+    "jobTitle" : "Partner",
+    "lastName" : "Auditor",
+    "firstName" : "Auvenir",
+    "password_salt" : "$2a$10$boqWtpVZ494jnH7drtPVMu",
+    "password" : "$2a$10$boqWtpVZ494jnH7drtPVMuqwXhErLcIcw9VxMbuZCpZdyWuRn.1j6",
+    "__v" : 1
+}</t>
+  </si>
+  <si>
+    <t>General Auditor</t>
+  </si>
+  <si>
+    <t>general.auditorthuan@vietnam-software.org</t>
+  </si>
+  <si>
+    <t>Auvenir</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4405e87847296323fab1"},
+    "userID" : { "$oid" : "59db4405e87847296323faaf"},
+    "firmID" : { "$oid" : "59db42c0e87847296323fa8c"},
+    "role" : "FIRM_USER",
+    "priority" : 8,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4405e87847296323fab0"},
+    "userID" : { "$oid" : "59db4405e87847296323faaf"},
+    "engagementID" : { "$oid" : "59db43b0e87847296323faa4"},
+    "role" : "GENERAL_AUDITOR",
+    "priority" : 2,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>adm.clientthuan@vietnam-software.org</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4373e87847296323fa9d"},
+    "userID" : { "$oid" : "59db4373e87847296323fa9b"},
+    "businessID" : { "$oid" : "59db4308e87847296323fa8f"},
+    "role" : "BUSINESS_ADMIN",
+    "priority" : 9,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4373e87847296323fa9b"},
+    "email" : "adm.clientthuan@vietnam-software.org",
+    "type" : "CLIENT",
+    "status" : "ACTIVE",
+    "locale" : "en-US",
+    "notification" : {
+        "SMSVerified" : false,
+        "SMSEnabled" : false,
+        "day" : null,
+        "time" : null,
+        "frequency" : "IMMEDIATELY",
+        "content" : "JUSTME"
+    },
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "passwordLockout" : {
+        "expires" : null,
+        "failedAttempts" : 0
+    },
+    "auth" : {
+        "id" : "tqd4FFFYMPz7-1F8L4F7P6L9h",
+        "access" : {
+            "expires" : {"$date":"2017-10-10T03:00:21.040Z"}
+        }
+    },
+    "referral" : "",
+    "agreements" : [ 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-10T03:00:00.335Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-10T03:00:00.335Z"}
+        }, 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-10T03:00:00.335Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-10T03:00:00.335Z"}
+        }
+    ],
+    "integrations" : [],
+    "verified" : false,
+    "passwordResetRequired" : false,
+    "lastOnboardedEID" : "",
+    "skipOnboard" : false,
+    "lastLogin" : {"$date":"2017-10-10T03:00:22.803Z"},
+    "dateCreated" : {"$date":"2017-10-10T03:02:34.569Z"},
+    "phone" : "234-567-8999",
+    "jobTitle" : "IT",
+    "lastName" : "Client",
+    "firstName" : "Admin",
+    "password_salt" : "$2a$10$NFJuTVV4yzVH9vXAvUP.pO",
+    "password" : "$2a$10$NFJuTVV4yzVH9vXAvUP.pOfhVbcGpRavQ4NUNHgc66r7fd7Aicu/y",
+    "__v" : 4
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4373e87847296323fa9c"},
+    "userID" : { "$oid" : "59db4373e87847296323fa9b"},
+    "engagementID" : { "$oid" : "59db4308e87847296323fa90"},
+    "role" : "LEAD_CLIENT",
+    "priority" : 3,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db43cee87847296323faa9"},
+    "userID" : { "$oid" : "59db4373e87847296323fa9b"},
+    "engagementID" : { "$oid" : "59db43b0e87847296323faa4"},
+    "role" : "BUSINESS_ADMIN",
+    "priority" : 9,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>Engagement1 Admin role mapping Json</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db4373e87847296323fa9e"},
+    "userID" : { "$oid" : "59db4373e87847296323fa9b"},
+    "engagementID" : { "$oid" : "59db4308e87847296323fa90"},
+    "role" : "BUSINESS_ADMIN",
+    "priority" : 9,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>lead.clientthuan@vietnam-software.org</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db444fe87847296323fab8"},
+    "email" : "lead.clientthuan@vietnam-software.org",
+    "type" : "CLIENT",
+    "status" : "ACTIVE",
+    "locale" : "en-US",
+    "notification" : {
+        "SMSVerified" : false,
+        "SMSEnabled" : false,
+        "day" : null,
+        "time" : null,
+        "frequency" : "IMMEDIATELY",
+        "content" : "JUSTME"
+    },
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "passwordLockout" : {
+        "expires" : null,
+        "failedAttempts" : 0
+    },
+    "auth" : {
+        "id" : "VGwqD8iOO65m-5cqYQ8N2VYkn",
+        "access" : {
+            "expires" : {"$date":"2017-10-10T03:00:55.268Z"}
+        }
+    },
+    "referral" : "",
+    "agreements" : [ 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:58:04.477Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:58:04.477Z"}
+        }, 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:58:04.477Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:58:04.477Z"}
+        }
+    ],
+    "integrations" : [],
+    "verified" : false,
+    "passwordResetRequired" : false,
+    "lastOnboardedEID" : "",
+    "skipOnboard" : false,
+    "lastLogin" : {"$date":"2017-10-10T03:00:58.744Z"},
+    "dateCreated" : {"$date":"2017-10-09T11:58:31.478Z"},
+    "phone" : "123-456-7899",
+    "jobTitle" : "IT",
+    "lastName" : "Client",
+    "firstName" : "Lead",
+    "password_salt" : "$2a$10$pCWmCS7d2yLSWfDIFtnHbu",
+    "password" : "$2a$10$pCWmCS7d2yLSWfDIFtnHbu.sMfbwYR4QcDL3U.jsjxf8oAYOJT2Yq",
+    "__v" : 1
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db444fe87847296323faba"},
+    "userID" : { "$oid" : "59db444fe87847296323fab8"},
+    "businessID" : { "$oid" : "59db4308e87847296323fa8f"},
+    "role" : "BUSINESS_USER",
+    "priority" : 10,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db444fe87847296323fab9"},
+    "userID" : { "$oid" : "59db444fe87847296323fab8"},
+    "engagementID" : { "$oid" : "59db43b0e87847296323faa4"},
+    "role" : "LEAD_CLIENT",
+    "priority" : 3,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db44b4e87847296323fac4"},
+    "email" : "general.clientthuan@vietnam-software.org",
+    "type" : "CLIENT",
+    "status" : "ACTIVE",
+    "locale" : "en-US",
+    "notification" : {
+        "SMSVerified" : false,
+        "SMSEnabled" : false,
+        "day" : null,
+        "time" : null,
+        "frequency" : "IMMEDIATELY",
+        "content" : "JUSTME"
+    },
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "passwordLockout" : {
+        "expires" : null,
+        "failedAttempts" : 0
+    },
+    "auth" : {
+        "id" : "qCxr1NUlmnTh-tv2XJB5hjulY",
+        "access" : {
+            "expires" : {"$date":"2017-10-11T04:25:29.465Z"}
+        }
+    },
+    "referral" : "",
+    "agreements" : [ 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:59:48.218Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:59:48.218Z"}
+        }, 
+        {
+            "agreementID" : "TAC-0",
+            "timeStamp" : {"$date":"2017-10-09T11:59:48.218Z"}
+        }, 
+        {
+            "agreementID" : "PP-0",
+            "timeStamp" : {"$date":"2017-10-09T11:59:48.218Z"}
+        }
+    ],
+    "integrations" : [],
+    "verified" : false,
+    "passwordResetRequired" : false,
+    "lastOnboardedEID" : "",
+    "skipOnboard" : false,
+    "lastLogin" : {"$date":"2017-10-11T04:25:32.788Z"},
+    "dateCreated" : {"$date":"2017-10-09T12:00:15.446Z"},
+    "phone" : "123-456-7899",
+    "jobTitle" : "IT",
+    "lastName" : "Client",
+    "firstName" : "General",
+    "password_salt" : "$2a$10$9xaz0.Lw6BjaP3XbmPvc1u",
+    "password" : "$2a$10$9xaz0.Lw6BjaP3XbmPvc1u3kupcvz5spGF7Gc/zNVReyDZoysnNLW",
+    "__v" : 1
+}</t>
+  </si>
+  <si>
+    <t>General Client</t>
+  </si>
+  <si>
+    <t>general.clientthuan@vietnam-software.org</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db44b4e87847296323fac6"},
+    "userID" : { "$oid" : "59db44b4e87847296323fac4"},
+    "businessID" : { "$oid" : "59db4308e87847296323fa8f"},
+    "role" : "BUSINESS_USER",
+    "priority" : 10,
+    "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "59db44b4e87847296323fac5"},
+    "userID" : { "$oid" : "59db44b4e87847296323fac4"},
+    "engagementID" : { "$oid" : "59db43b0e87847296323faa4"},
+    "role" : "GENERAL_CLIENT",
+    "priority" : 4,
+    "__v" : 0
+}</t>
   </si>
 </sst>
 </file>
@@ -2629,7 +3400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2785,9 +3556,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2795,6 +3563,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2809,11 +3580,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8102,186 +8876,328 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="37" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="37"/>
-    <col min="5" max="5" width="9.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="37" customWidth="1"/>
-    <col min="10" max="10" width="20" style="37" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" style="37" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" style="37" customWidth="1"/>
-    <col min="13" max="13" width="21" style="37" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="37"/>
+    <col min="1" max="1" width="16.28515625" style="87" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="87" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="87" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="87"/>
+    <col min="5" max="5" width="9.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="87" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="87" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="87" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="87" customWidth="1"/>
+    <col min="10" max="10" width="20" style="87" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" style="87" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="87" customWidth="1"/>
+    <col min="13" max="13" width="21" style="87" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="87" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="87"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="87" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="87" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="87" t="s">
         <v>228</v>
       </c>
       <c r="F1" s="87" t="s">
-        <v>227</v>
-      </c>
-      <c r="G1" s="87" t="s">
-        <v>634</v>
-      </c>
-      <c r="H1" s="87" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="88" t="s">
+        <v>656</v>
+      </c>
+      <c r="H1" s="88" t="s">
+        <v>657</v>
+      </c>
+      <c r="I1" s="88" t="s">
+        <v>677</v>
+      </c>
+      <c r="J1" s="87" t="s">
+        <v>221</v>
+      </c>
+      <c r="K1" s="88" t="s">
+        <v>645</v>
+      </c>
+      <c r="L1" s="88" t="s">
+        <v>649</v>
+      </c>
+      <c r="M1" s="88" t="s">
+        <v>653</v>
+      </c>
+      <c r="N1" s="88" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="87" t="s">
+        <v>504</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>557</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="87" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="87" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>632</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>639</v>
+      </c>
+      <c r="H2" s="87" t="s">
+        <v>638</v>
+      </c>
+      <c r="J2" s="87" t="s">
+        <v>214</v>
+      </c>
+      <c r="K2" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="87" t="s">
+        <v>505</v>
+      </c>
+      <c r="B3" s="89" t="s">
+        <v>503</v>
+      </c>
+      <c r="C3" s="87" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="87" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="87" t="s">
+        <v>633</v>
+      </c>
+      <c r="G3" s="87" t="s">
+        <v>641</v>
+      </c>
+      <c r="H3" s="87" t="s">
+        <v>637</v>
+      </c>
+      <c r="J3" s="87" t="s">
+        <v>208</v>
+      </c>
+      <c r="K3" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="87" t="s">
+        <v>509</v>
+      </c>
+      <c r="B4" s="89" t="s">
+        <v>646</v>
+      </c>
+      <c r="C4" s="87" t="s">
+        <v>644</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" s="87" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" s="87" t="s">
+        <v>648</v>
+      </c>
+      <c r="G4" s="87" t="s">
+        <v>662</v>
+      </c>
+      <c r="H4" s="87" t="s">
+        <v>663</v>
+      </c>
+      <c r="I4" s="87" t="s">
+        <v>664</v>
+      </c>
+      <c r="J4" s="87" t="s">
+        <v>650</v>
+      </c>
+      <c r="K4" s="87" t="s">
+        <v>647</v>
+      </c>
+      <c r="L4" s="87" t="s">
+        <v>651</v>
+      </c>
+      <c r="M4" s="87" t="s">
         <v>652</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>222</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>221</v>
-      </c>
-      <c r="K1" s="87" t="s">
-        <v>645</v>
-      </c>
-      <c r="L1" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="87" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>504</v>
-      </c>
-      <c r="B2" s="88" t="s">
-        <v>557</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>636</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>639</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>638</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>632</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>549</v>
-      </c>
-      <c r="M2" s="37" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>505</v>
-      </c>
-      <c r="B3" s="88" t="s">
-        <v>503</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>640</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>641</v>
-      </c>
-      <c r="H3" s="37" t="s">
-        <v>637</v>
-      </c>
-      <c r="I3" s="37" t="s">
-        <v>633</v>
-      </c>
-      <c r="J3" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="K3" s="37" t="s">
-        <v>643</v>
-      </c>
-      <c r="L3" s="37" t="s">
-        <v>549</v>
-      </c>
-      <c r="M3" s="37" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>509</v>
-      </c>
-      <c r="B4" s="88" t="s">
-        <v>646</v>
-      </c>
-      <c r="C4" s="37" t="s">
+    </row>
+    <row r="5" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="87" t="s">
+        <v>512</v>
+      </c>
+      <c r="B5" s="89" t="s">
+        <v>654</v>
+      </c>
+      <c r="C5" s="87" t="s">
         <v>644</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D5" s="87" t="s">
+        <v>586</v>
+      </c>
+      <c r="E5" s="87" t="s">
+        <v>234</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>655</v>
+      </c>
+      <c r="G5" s="87" t="s">
+        <v>660</v>
+      </c>
+      <c r="H5" s="87" t="s">
+        <v>661</v>
+      </c>
+      <c r="K5" s="87" t="s">
+        <v>658</v>
+      </c>
+      <c r="N5" s="87" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="87" t="s">
+        <v>667</v>
+      </c>
+      <c r="B6" s="89" t="s">
+        <v>668</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>644</v>
+      </c>
+      <c r="D6" s="87" t="s">
+        <v>669</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" s="87" t="s">
+        <v>666</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>671</v>
+      </c>
+      <c r="K6" s="87" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="87" t="s">
+        <v>516</v>
+      </c>
+      <c r="B7" s="89" t="s">
+        <v>672</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="87" t="s">
         <v>233</v>
       </c>
-      <c r="E4" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>647</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>651</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>649</v>
-      </c>
-      <c r="J4" s="37" t="s">
-        <v>650</v>
-      </c>
-      <c r="K4" s="37" t="s">
-        <v>648</v>
+      <c r="E7" s="87" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" s="87" t="s">
+        <v>674</v>
+      </c>
+      <c r="G7" s="87" t="s">
+        <v>675</v>
+      </c>
+      <c r="H7" s="87" t="s">
+        <v>676</v>
+      </c>
+      <c r="I7" s="87" t="s">
+        <v>678</v>
+      </c>
+      <c r="K7" s="87" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="s">
+        <v>519</v>
+      </c>
+      <c r="B8" s="89" t="s">
+        <v>679</v>
+      </c>
+      <c r="C8" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="87" t="s">
+        <v>586</v>
+      </c>
+      <c r="E8" s="87" t="s">
+        <v>235</v>
+      </c>
+      <c r="F8" s="87" t="s">
+        <v>680</v>
+      </c>
+      <c r="H8" s="87" t="s">
+        <v>682</v>
+      </c>
+      <c r="K8" s="87" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="87" t="s">
+        <v>684</v>
+      </c>
+      <c r="B9" s="89" t="s">
+        <v>685</v>
+      </c>
+      <c r="C9" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="87" t="s">
+        <v>686</v>
+      </c>
+      <c r="E9" s="87" t="s">
+        <v>235</v>
+      </c>
+      <c r="F9" s="87" t="s">
+        <v>683</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>688</v>
+      </c>
+      <c r="K9" s="87" t="s">
+        <v>687</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9012,22 +9928,22 @@
       <c r="Q1" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="79" t="s">
+      <c r="R1" s="82" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="79"/>
-      <c r="T1" s="82" t="s">
+      <c r="S1" s="82"/>
+      <c r="T1" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="80"/>
-      <c r="V1" s="79" t="s">
+      <c r="U1" s="79"/>
+      <c r="V1" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="80" t="s">
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="79" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="83" t="s">
@@ -9079,8 +9995,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="81"/>
-      <c r="AB2" s="81"/>
+      <c r="AA2" s="80"/>
+      <c r="AB2" s="80"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -9136,17 +10052,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -9157,6 +10062,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor code - create Admin and Super Admin user.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="699">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -3187,6 +3187,215 @@
     "role" : "GENERAL_CLIENT",
     "priority" : 4,
     "__v" : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "5922b8ae7d63f54b5a01760a"},
+    "status" : "ACTIVE",
+    "email" : "chr.auvenirad@gmail.com",
+    "type" : "SUPER ADMIN",
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "fileUpload" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "referral" : "",
+    "agreements" : [],
+    "integrations" : [],
+    "verified" : false,
+    "phone" : "",
+    "jobTitle" : "auditor",
+    "lastName" : "tran",
+    "firstName" : "doai",
+    "__v" : 0,
+    "lastLogin" : {"$date":"2017-05-23T07:37:56.456Z"},
+    "dateCreated" : {"$date":"2017-10-09 11:53:51.258Z"},
+    "auth" : {
+        "id" : null,
+        "access" : {
+            "expires" : {"$date":"2017-05-23T07:37:56.456Z"}
+        }
+    },
+    "password" : "$2a$10$KbMHrucfPvB4PK4t5Oz0Xey5L.b9OPq5eBUZTaPBexzWzfblZysn2",
+    "password_salt" : "$2a$10$KbMHrucfPvB4PK4t5Oz0Xe"
+}</t>
+  </si>
+  <si>
+    <t>doai</t>
+  </si>
+  <si>
+    <t>tran</t>
+  </si>
+  <si>
+    <t>SUPER ADMIN</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "58f707a6004d69fc2aeb8e4a"},
+    "status" : "ACTIVE",
+    "email" : "chr.adm.auvenir@gmail.com",
+    "type" : "ADMIN",
+    "notifications" : {
+        "todoCompleted" : {
+            "email" : false
+        },
+        "fileUpload" : {
+            "email" : false
+        },
+        "newRequest" : {
+            "email" : false
+        },
+        "newComment" : {
+            "email" : false
+        },
+        "newTodo" : {
+            "email" : false
+        },
+        "documentUploaded" : {
+            "email" : false
+        },
+        "joinEngagement" : {
+            "email" : false
+        },
+        "engagementInvite" : {
+            "email" : false
+        }
+    },
+    "referral" : "",
+    "agreements" : [],
+    "integrations" : [],
+    "verified" : false,
+    "phone" : "",
+    "jobTitle" : "",
+    "lastName" : "nguyen",
+    "firstName" : "cuong",
+    "__v" : 0,
+    "lastLogin" : {"$date":"2017-10-11T10:00:27.294Z"},
+    "dateCreated" : null,
+    "auth" : {
+        "id" : null,
+        "access" : {
+            "expires" : {"$date":"2017-10-11T10:00:23.756Z"}
+        }
+    },
+    "password" : "$2a$10$KbMHrucfPvB4PK4t5Oz0Xey5L.b9OPq5eBUZTaPBexzWzfblZysn2",
+    "password_salt" : "$2a$10$KbMHrucfPvB4PK4t5Oz0Xe",
+    "locale" : "en-CA",
+    "notification" : {
+        "content" : "JUSTME",
+        "frequency" : "IMMEDIATELY"
+    },
+    "passwordLockout" : {
+        "failedAttempts" : 0
+    },
+    "skipOnboard" : true
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "5922b8ae7d63f54b5a01760b"},
+    "name" : "SUPER ADMIN",
+    "address" : {
+        "country" : "CA",
+        "postalCode" : "K3G4P8",
+        "stateProvince" : "Quebec",
+        "city" : "Toronto",
+        "streetAddress" : "123 Hoang Van Thu",
+        "unit" : "12345"
+    },
+    "memberID" : "3215",
+    "previousName" : "",
+    "nameChange" : false,
+    "logoDisplayAgreed" : false,
+    "affiliatedFirms" : [],
+    "affiliated" : false,
+    "phone" : "123456-7890",
+    "size" : "1",
+    "website" : "titancorpvn.com",
+    "logo" : "",
+    "acl" : [
+  {
+            "id" : { "$oid" : "5922b8ae7d63f54b5a01760a"},
+            "admin" : true
+        }
+ ],
+    "__v" : 1
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "58f707a6004d69fc2aeb8e4b"},
+    "name" : "ADMIN USER",
+    "address" : {
+        "country" : "CA",
+        "postalCode" : "K3G4P8",
+        "stateProvince" : "Quebec",
+        "city" : "Toronto",
+        "streetAddress" : "123 Hoang Van Thu",
+        "unit" : "12345"
+    },
+    "memberID" : "3215",
+    "previousName" : "",
+    "nameChange" : false,
+    "logoDisplayAgreed" : false,
+    "affiliatedFirms" : [],
+    "affiliated" : false,
+    "phone" : "123456-7890",
+    "size" : "1",
+    "website" : "titancorpvn.com",
+    "logo" : "",
+    "acl" : [
+  {
+            "id" : { "$oid" : "58f707a6004d69fc2aeb8e4a"},
+            "admin" : true
+        }
+ ],
+    "__v" : 1
+}</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "5922b8ae7d63f54b5a01760c"},
+    "role" : "AUVY_ADMIN",
+    "priority" : 7,
+    "__v" : 0,
+    "userID" : { "$oid" : "5922b8ae7d63f54b5a01760a"},
+    "firmID" : { "$oid" : "5922b8ae7d63f54b5a01760b"}
+}</t>
+  </si>
+  <si>
+    <t>{
+    "_id" : { "$oid" : "58f707a6004d69fc2aeb8e4c"},
+    "role" : "AUVY_ADMIN",
+    "priority" : 7,
+    "__v" : 0,
+    "userID" : { "$oid" : "58f707a6004d69fc2aeb8e4a"},
+    "firmID" : { "$oid" : "58f707a6004d69fc2aeb8e4b"}
 }</t>
   </si>
 </sst>
@@ -3553,8 +3762,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3563,9 +3784,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3579,15 +3797,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8596,7 +8805,7 @@
   <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8613,7 +8822,7 @@
     <col min="11" max="11" width="29.5703125" customWidth="1"/>
     <col min="12" max="12" width="23.85546875" customWidth="1"/>
     <col min="13" max="13" width="28.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" customWidth="1"/>
     <col min="15" max="15" width="27.5703125" style="75" customWidth="1"/>
     <col min="17" max="17" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -8879,313 +9088,301 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="87" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="87" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="87"/>
-    <col min="5" max="5" width="9.7109375" style="87" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" style="87" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="87" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" style="87" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="87" customWidth="1"/>
-    <col min="10" max="10" width="20" style="87" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" style="87" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" style="87" customWidth="1"/>
-    <col min="13" max="13" width="21" style="87" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="87" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="87"/>
+    <col min="1" max="1" width="16.28515625" style="78" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="78" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="78"/>
+    <col min="5" max="5" width="9.7109375" style="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="78" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="78" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="78" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="78" customWidth="1"/>
+    <col min="10" max="10" width="20" style="78" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" style="78" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="78" customWidth="1"/>
+    <col min="13" max="13" width="21" style="78" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="78" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="78"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="78" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="78" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="78" t="s">
         <v>228</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="78" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="79" t="s">
         <v>656</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="79" t="s">
         <v>657</v>
       </c>
-      <c r="I1" s="88" t="s">
+      <c r="I1" s="79" t="s">
         <v>677</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="78" t="s">
         <v>221</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="K1" s="79" t="s">
         <v>645</v>
       </c>
-      <c r="L1" s="88" t="s">
+      <c r="L1" s="79" t="s">
         <v>649</v>
       </c>
-      <c r="M1" s="88" t="s">
+      <c r="M1" s="79" t="s">
         <v>653</v>
       </c>
-      <c r="N1" s="88" t="s">
+      <c r="N1" s="79" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
-        <v>504</v>
-      </c>
-      <c r="B2" s="89" t="s">
+    <row r="2" spans="1:14" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" s="80" t="s">
         <v>557</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="78" t="s">
+        <v>692</v>
+      </c>
+      <c r="D2" s="78" t="s">
+        <v>690</v>
+      </c>
+      <c r="E2" s="78" t="s">
+        <v>691</v>
+      </c>
+      <c r="F2" s="78" t="s">
+        <v>689</v>
+      </c>
+      <c r="J2" s="78" t="s">
+        <v>694</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="78" t="s">
+        <v>696</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>503</v>
+      </c>
+      <c r="C3" s="78" t="s">
         <v>220</v>
       </c>
-      <c r="D2" s="87" t="s">
+      <c r="D3" s="78" t="s">
         <v>219</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E3" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="87" t="s">
-        <v>632</v>
-      </c>
-      <c r="G2" s="87" t="s">
-        <v>639</v>
-      </c>
-      <c r="H2" s="87" t="s">
-        <v>638</v>
-      </c>
-      <c r="J2" s="87" t="s">
-        <v>214</v>
-      </c>
-      <c r="K2" s="87" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
-        <v>505</v>
-      </c>
-      <c r="B3" s="89" t="s">
-        <v>503</v>
-      </c>
-      <c r="C3" s="87" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="87" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" s="87" t="s">
-        <v>212</v>
-      </c>
-      <c r="F3" s="87" t="s">
-        <v>633</v>
-      </c>
-      <c r="G3" s="87" t="s">
-        <v>641</v>
-      </c>
-      <c r="H3" s="87" t="s">
-        <v>637</v>
-      </c>
-      <c r="J3" s="87" t="s">
-        <v>208</v>
-      </c>
-      <c r="K3" s="87" t="s">
-        <v>643</v>
+      <c r="F3" s="78" t="s">
+        <v>693</v>
+      </c>
+      <c r="J3" s="78" t="s">
+        <v>695</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="78" t="s">
         <v>509</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="80" t="s">
         <v>646</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="78" t="s">
         <v>644</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="78" t="s">
         <v>233</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="78" t="s">
         <v>234</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="78" t="s">
         <v>648</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="78" t="s">
         <v>662</v>
       </c>
-      <c r="H4" s="87" t="s">
+      <c r="H4" s="78" t="s">
         <v>663</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="78" t="s">
         <v>664</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="78" t="s">
         <v>650</v>
       </c>
-      <c r="K4" s="87" t="s">
+      <c r="K4" s="78" t="s">
         <v>647</v>
       </c>
-      <c r="L4" s="87" t="s">
+      <c r="L4" s="78" t="s">
         <v>651</v>
       </c>
-      <c r="M4" s="87" t="s">
+      <c r="M4" s="78" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="78" t="s">
         <v>512</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="80" t="s">
         <v>654</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="78" t="s">
         <v>644</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="D5" s="78" t="s">
         <v>586</v>
       </c>
-      <c r="E5" s="87" t="s">
+      <c r="E5" s="78" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="87" t="s">
+      <c r="F5" s="78" t="s">
         <v>655</v>
       </c>
-      <c r="G5" s="87" t="s">
+      <c r="G5" s="78" t="s">
         <v>660</v>
       </c>
-      <c r="H5" s="87" t="s">
+      <c r="H5" s="78" t="s">
         <v>661</v>
       </c>
-      <c r="K5" s="87" t="s">
+      <c r="K5" s="78" t="s">
         <v>658</v>
       </c>
-      <c r="N5" s="87" t="s">
+      <c r="N5" s="78" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="78" t="s">
         <v>667</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="80" t="s">
         <v>668</v>
       </c>
-      <c r="C6" s="87" t="s">
+      <c r="C6" s="78" t="s">
         <v>644</v>
       </c>
-      <c r="D6" s="87" t="s">
+      <c r="D6" s="78" t="s">
         <v>669</v>
       </c>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="78" t="s">
         <v>234</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="78" t="s">
         <v>666</v>
       </c>
-      <c r="H6" s="87" t="s">
+      <c r="H6" s="78" t="s">
         <v>671</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K6" s="78" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="78" t="s">
         <v>516</v>
       </c>
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="80" t="s">
         <v>672</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="87" t="s">
+      <c r="D7" s="78" t="s">
         <v>233</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="78" t="s">
         <v>235</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="78" t="s">
         <v>674</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="78" t="s">
         <v>675</v>
       </c>
-      <c r="H7" s="87" t="s">
+      <c r="H7" s="78" t="s">
         <v>676</v>
       </c>
-      <c r="I7" s="87" t="s">
+      <c r="I7" s="78" t="s">
         <v>678</v>
       </c>
-      <c r="K7" s="87" t="s">
+      <c r="K7" s="78" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="78" t="s">
         <v>519</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="80" t="s">
         <v>679</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="87" t="s">
+      <c r="D8" s="78" t="s">
         <v>586</v>
       </c>
-      <c r="E8" s="87" t="s">
+      <c r="E8" s="78" t="s">
         <v>235</v>
       </c>
-      <c r="F8" s="87" t="s">
+      <c r="F8" s="78" t="s">
         <v>680</v>
       </c>
-      <c r="H8" s="87" t="s">
+      <c r="H8" s="78" t="s">
         <v>682</v>
       </c>
-      <c r="K8" s="87" t="s">
+      <c r="K8" s="78" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="78" t="s">
         <v>684</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="80" t="s">
         <v>685</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="78" t="s">
         <v>686</v>
       </c>
-      <c r="E9" s="87" t="s">
+      <c r="E9" s="78" t="s">
         <v>235</v>
       </c>
-      <c r="F9" s="87" t="s">
+      <c r="F9" s="78" t="s">
         <v>683</v>
       </c>
-      <c r="H9" s="87" t="s">
+      <c r="H9" s="78" t="s">
         <v>688</v>
       </c>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="78" t="s">
         <v>687</v>
       </c>
     </row>
@@ -9880,62 +10077,62 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="81" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="78" t="s">
+      <c r="G1" s="81" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="78" t="s">
+      <c r="H1" s="81" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="78" t="s">
+      <c r="I1" s="81" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="J1" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="78" t="s">
+      <c r="K1" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="L1" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="M1" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="78" t="s">
+      <c r="N1" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="78" t="s">
+      <c r="O1" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="78" t="s">
+      <c r="P1" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="Q1" s="81" t="s">
         <v>143</v>
       </c>
       <c r="R1" s="82" t="s">
         <v>197</v>
       </c>
       <c r="S1" s="82"/>
-      <c r="T1" s="81" t="s">
+      <c r="T1" s="85" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="79"/>
+      <c r="U1" s="83"/>
       <c r="V1" s="82" t="s">
         <v>195</v>
       </c>
@@ -9943,31 +10140,31 @@
       <c r="X1" s="82"/>
       <c r="Y1" s="82"/>
       <c r="Z1" s="82"/>
-      <c r="AA1" s="79" t="s">
+      <c r="AA1" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="83" t="s">
+      <c r="AB1" s="86" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -9995,8 +10192,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="80"/>
-      <c r="AB2" s="80"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -10052,6 +10249,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -10062,17 +10270,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10200,11 +10397,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="86"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="89"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>

</xml_diff>